<commit_message>
New Character Sheets, small changes
</commit_message>
<xml_diff>
--- a/Tokens/Tokens.xlsx
+++ b/Tokens/Tokens.xlsx
@@ -42,12 +42,6 @@
     <t>Invisibility</t>
   </si>
   <si>
-    <t>Burning</t>
-  </si>
-  <si>
-    <t>Salamanders</t>
-  </si>
-  <si>
     <t>Gal Vorbak</t>
   </si>
   <si>
@@ -85,6 +79,12 @@
   </si>
   <si>
     <t>Rending</t>
+  </si>
+  <si>
+    <t>Burning/Corrosion</t>
+  </si>
+  <si>
+    <t>Salamanders/Nurgle</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +488,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -499,7 +499,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -510,88 +510,88 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>